<commit_message>
updated data till 20th Feb
</commit_message>
<xml_diff>
--- a/data/pilot_data/Statistics-8arm_pilot.xlsx
+++ b/data/pilot_data/Statistics-8arm_pilot.xlsx
@@ -11457,6 +11457,1334 @@
         <v>37443.2</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Trial    96</t>
+        </is>
+      </c>
+      <c r="B99">
+        <v>1465.93</v>
+      </c>
+      <c r="C99">
+        <v>10.8856</v>
+      </c>
+      <c r="D99">
+        <v>17</v>
+      </c>
+      <c r="E99">
+        <v>138.1</v>
+      </c>
+      <c r="F99">
+        <v>1.1</v>
+      </c>
+      <c r="G99">
+        <v>20</v>
+      </c>
+      <c r="H99">
+        <v>45.6666</v>
+      </c>
+      <c r="I99">
+        <v>2.2</v>
+      </c>
+      <c r="J99">
+        <v>11</v>
+      </c>
+      <c r="K99">
+        <v>19.9</v>
+      </c>
+      <c r="L99">
+        <v>1.1</v>
+      </c>
+      <c r="M99">
+        <v>8</v>
+      </c>
+      <c r="N99">
+        <v>5.76666</v>
+      </c>
+      <c r="O99">
+        <v>2.1</v>
+      </c>
+      <c r="P99">
+        <v>5</v>
+      </c>
+      <c r="Q99">
+        <v>20.1666</v>
+      </c>
+      <c r="R99">
+        <v>48.3666</v>
+      </c>
+      <c r="S99">
+        <v>3</v>
+      </c>
+      <c r="T99">
+        <v>2.1</v>
+      </c>
+      <c r="U99">
+        <v>3.46666</v>
+      </c>
+      <c r="V99">
+        <v>3</v>
+      </c>
+      <c r="W99">
+        <v>17.1</v>
+      </c>
+      <c r="X99">
+        <v>71.7333</v>
+      </c>
+      <c r="Y99">
+        <v>2</v>
+      </c>
+      <c r="Z99">
+        <v>20.3</v>
+      </c>
+      <c r="AA99">
+        <v>35.1333</v>
+      </c>
+      <c r="AB99">
+        <v>3</v>
+      </c>
+      <c r="AC99">
+        <v>2.66666</v>
+      </c>
+      <c r="AD99">
+        <v>103.033</v>
+      </c>
+      <c r="AE99">
+        <v>4</v>
+      </c>
+      <c r="AF99">
+        <v>2.93333</v>
+      </c>
+      <c r="AG99">
+        <v>9.76666</v>
+      </c>
+      <c r="AH99">
+        <v>12.1581</v>
+      </c>
+      <c r="AI99">
+        <v>49483.4</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Trial    97</t>
+        </is>
+      </c>
+      <c r="B100">
+        <v>1654.02</v>
+      </c>
+      <c r="C100">
+        <v>14.5047</v>
+      </c>
+      <c r="D100">
+        <v>26</v>
+      </c>
+      <c r="E100">
+        <v>119.6</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>19</v>
+      </c>
+      <c r="H100">
+        <v>28.5333</v>
+      </c>
+      <c r="I100">
+        <v>3.73333</v>
+      </c>
+      <c r="J100">
+        <v>13</v>
+      </c>
+      <c r="K100">
+        <v>11.5333</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>12</v>
+      </c>
+      <c r="N100">
+        <v>14.8</v>
+      </c>
+      <c r="O100">
+        <v>2.36666</v>
+      </c>
+      <c r="P100">
+        <v>11</v>
+      </c>
+      <c r="Q100">
+        <v>15.3</v>
+      </c>
+      <c r="R100">
+        <v>2.83333</v>
+      </c>
+      <c r="S100">
+        <v>5</v>
+      </c>
+      <c r="T100">
+        <v>14.0667</v>
+      </c>
+      <c r="U100">
+        <v>3.9</v>
+      </c>
+      <c r="V100">
+        <v>4</v>
+      </c>
+      <c r="W100">
+        <v>17.2333</v>
+      </c>
+      <c r="X100">
+        <v>46.5666</v>
+      </c>
+      <c r="Y100">
+        <v>3</v>
+      </c>
+      <c r="Z100">
+        <v>13.2333</v>
+      </c>
+      <c r="AA100">
+        <v>10.2</v>
+      </c>
+      <c r="AB100">
+        <v>3</v>
+      </c>
+      <c r="AC100">
+        <v>1.9</v>
+      </c>
+      <c r="AD100">
+        <v>73.2999</v>
+      </c>
+      <c r="AE100">
+        <v>5</v>
+      </c>
+      <c r="AF100">
+        <v>1.06667</v>
+      </c>
+      <c r="AG100">
+        <v>14.8667</v>
+      </c>
+      <c r="AH100">
+        <v>13.2942</v>
+      </c>
+      <c r="AI100">
+        <v>46117.5</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Trial    98</t>
+        </is>
+      </c>
+      <c r="B101">
+        <v>1557.9</v>
+      </c>
+      <c r="C101">
+        <v>11.6232</v>
+      </c>
+      <c r="D101">
+        <v>24</v>
+      </c>
+      <c r="E101">
+        <v>138.833</v>
+      </c>
+      <c r="F101">
+        <v>3.4</v>
+      </c>
+      <c r="G101">
+        <v>22</v>
+      </c>
+      <c r="H101">
+        <v>46.0666</v>
+      </c>
+      <c r="I101">
+        <v>3.8</v>
+      </c>
+      <c r="J101">
+        <v>12</v>
+      </c>
+      <c r="K101">
+        <v>11</v>
+      </c>
+      <c r="L101">
+        <v>29.2</v>
+      </c>
+      <c r="M101">
+        <v>11</v>
+      </c>
+      <c r="N101">
+        <v>9.36666</v>
+      </c>
+      <c r="O101">
+        <v>3.4</v>
+      </c>
+      <c r="P101">
+        <v>4</v>
+      </c>
+      <c r="Q101">
+        <v>25.6666</v>
+      </c>
+      <c r="R101">
+        <v>4.03333</v>
+      </c>
+      <c r="S101">
+        <v>4</v>
+      </c>
+      <c r="T101">
+        <v>11.2</v>
+      </c>
+      <c r="U101">
+        <v>5.29999</v>
+      </c>
+      <c r="V101">
+        <v>5</v>
+      </c>
+      <c r="W101">
+        <v>16.4333</v>
+      </c>
+      <c r="X101">
+        <v>8.59999</v>
+      </c>
+      <c r="Y101">
+        <v>1</v>
+      </c>
+      <c r="Z101">
+        <v>7.86666</v>
+      </c>
+      <c r="AA101">
+        <v>136.467</v>
+      </c>
+      <c r="AB101">
+        <v>4</v>
+      </c>
+      <c r="AC101">
+        <v>4.39999</v>
+      </c>
+      <c r="AD101">
+        <v>28.4333</v>
+      </c>
+      <c r="AE101">
+        <v>8</v>
+      </c>
+      <c r="AF101">
+        <v>5.13333</v>
+      </c>
+      <c r="AG101">
+        <v>29.0666</v>
+      </c>
+      <c r="AH101">
+        <v>11.6261</v>
+      </c>
+      <c r="AI101">
+        <v>47213.5</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Trial    99</t>
+        </is>
+      </c>
+      <c r="B102">
+        <v>2476.81</v>
+      </c>
+      <c r="C102">
+        <v>13.9381</v>
+      </c>
+      <c r="D102">
+        <v>28</v>
+      </c>
+      <c r="E102">
+        <v>182.5</v>
+      </c>
+      <c r="F102">
+        <v>1.53333</v>
+      </c>
+      <c r="G102">
+        <v>28</v>
+      </c>
+      <c r="H102">
+        <v>33.2333</v>
+      </c>
+      <c r="I102">
+        <v>5.13333</v>
+      </c>
+      <c r="J102">
+        <v>14</v>
+      </c>
+      <c r="K102">
+        <v>20.2666</v>
+      </c>
+      <c r="L102">
+        <v>1.53333</v>
+      </c>
+      <c r="M102">
+        <v>10</v>
+      </c>
+      <c r="N102">
+        <v>25.0666</v>
+      </c>
+      <c r="O102">
+        <v>2.1</v>
+      </c>
+      <c r="P102">
+        <v>6</v>
+      </c>
+      <c r="Q102">
+        <v>22.1666</v>
+      </c>
+      <c r="R102">
+        <v>2.3</v>
+      </c>
+      <c r="S102">
+        <v>8</v>
+      </c>
+      <c r="T102">
+        <v>14.1</v>
+      </c>
+      <c r="U102">
+        <v>6.96666</v>
+      </c>
+      <c r="V102">
+        <v>13</v>
+      </c>
+      <c r="W102">
+        <v>44.3666</v>
+      </c>
+      <c r="X102">
+        <v>6.19999</v>
+      </c>
+      <c r="Y102">
+        <v>2</v>
+      </c>
+      <c r="Z102">
+        <v>13.2667</v>
+      </c>
+      <c r="AA102">
+        <v>28.3666</v>
+      </c>
+      <c r="AB102">
+        <v>3</v>
+      </c>
+      <c r="AC102">
+        <v>2.13333</v>
+      </c>
+      <c r="AD102">
+        <v>110.7</v>
+      </c>
+      <c r="AE102">
+        <v>5</v>
+      </c>
+      <c r="AF102">
+        <v>5.89999</v>
+      </c>
+      <c r="AG102">
+        <v>35.7666</v>
+      </c>
+      <c r="AH102">
+        <v>15.8732</v>
+      </c>
+      <c r="AI102">
+        <v>85223.4</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Trial   100</t>
+        </is>
+      </c>
+      <c r="B103">
+        <v>1045.09</v>
+      </c>
+      <c r="C103">
+        <v>11.3844</v>
+      </c>
+      <c r="D103">
+        <v>19</v>
+      </c>
+      <c r="E103">
+        <v>94.6332</v>
+      </c>
+      <c r="F103">
+        <v>2.3</v>
+      </c>
+      <c r="G103">
+        <v>13</v>
+      </c>
+      <c r="H103">
+        <v>25.6</v>
+      </c>
+      <c r="I103">
+        <v>3.56666</v>
+      </c>
+      <c r="J103">
+        <v>9</v>
+      </c>
+      <c r="K103">
+        <v>14.2</v>
+      </c>
+      <c r="L103">
+        <v>2.3</v>
+      </c>
+      <c r="M103">
+        <v>8</v>
+      </c>
+      <c r="N103">
+        <v>14.4333</v>
+      </c>
+      <c r="O103">
+        <v>3.03333</v>
+      </c>
+      <c r="P103">
+        <v>1</v>
+      </c>
+      <c r="Q103">
+        <v>0.133333</v>
+      </c>
+      <c r="R103">
+        <v>3.4</v>
+      </c>
+      <c r="S103">
+        <v>4</v>
+      </c>
+      <c r="T103">
+        <v>11.0667</v>
+      </c>
+      <c r="U103">
+        <v>47.1333</v>
+      </c>
+      <c r="V103">
+        <v>5</v>
+      </c>
+      <c r="W103">
+        <v>17.2333</v>
+      </c>
+      <c r="X103">
+        <v>46.1666</v>
+      </c>
+      <c r="Y103">
+        <v>1</v>
+      </c>
+      <c r="Z103">
+        <v>8.16666</v>
+      </c>
+      <c r="AA103">
+        <v>81.3333</v>
+      </c>
+      <c r="AB103">
+        <v>1</v>
+      </c>
+      <c r="AC103">
+        <v>0.666666</v>
+      </c>
+      <c r="AD103">
+        <v>25.1666</v>
+      </c>
+      <c r="AE103">
+        <v>3</v>
+      </c>
+      <c r="AF103">
+        <v>2</v>
+      </c>
+      <c r="AG103">
+        <v>10.3667</v>
+      </c>
+      <c r="AH103">
+        <v>14.6768</v>
+      </c>
+      <c r="AI103">
+        <v>40757.5</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Trial   101</t>
+        </is>
+      </c>
+      <c r="B104">
+        <v>476.747</v>
+      </c>
+      <c r="C104">
+        <v>13.3543</v>
+      </c>
+      <c r="D104">
+        <v>8</v>
+      </c>
+      <c r="E104">
+        <v>37.1666</v>
+      </c>
+      <c r="F104">
+        <v>0.933332</v>
+      </c>
+      <c r="G104">
+        <v>6</v>
+      </c>
+      <c r="H104">
+        <v>4.23333</v>
+      </c>
+      <c r="I104">
+        <v>7.29999</v>
+      </c>
+      <c r="J104">
+        <v>4</v>
+      </c>
+      <c r="K104">
+        <v>6.29999</v>
+      </c>
+      <c r="L104">
+        <v>0.933332</v>
+      </c>
+      <c r="M104">
+        <v>7</v>
+      </c>
+      <c r="N104">
+        <v>9.76666</v>
+      </c>
+      <c r="O104">
+        <v>6.36666</v>
+      </c>
+      <c r="P104">
+        <v>2</v>
+      </c>
+      <c r="Q104">
+        <v>1.76666</v>
+      </c>
+      <c r="R104">
+        <v>6.83333</v>
+      </c>
+      <c r="S104">
+        <v>1</v>
+      </c>
+      <c r="T104">
+        <v>7.59999</v>
+      </c>
+      <c r="U104">
+        <v>27.2666</v>
+      </c>
+      <c r="V104">
+        <v>1</v>
+      </c>
+      <c r="W104">
+        <v>1.3</v>
+      </c>
+      <c r="X104">
+        <v>7.66666</v>
+      </c>
+      <c r="Y104">
+        <v>1</v>
+      </c>
+      <c r="Z104">
+        <v>5.76666</v>
+      </c>
+      <c r="AA104">
+        <v>35.6666</v>
+      </c>
+      <c r="AB104">
+        <v>0</v>
+      </c>
+      <c r="AC104">
+        <v>0</v>
+      </c>
+      <c r="AD104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE104">
+        <v>0</v>
+      </c>
+      <c r="AF104">
+        <v>0</v>
+      </c>
+      <c r="AG104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH104">
+        <v>19.0708</v>
+      </c>
+      <c r="AI104">
+        <v>20653.7</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Trial   102</t>
+        </is>
+      </c>
+      <c r="B105">
+        <v>821.037</v>
+      </c>
+      <c r="C105">
+        <v>13.7297</v>
+      </c>
+      <c r="D105">
+        <v>14</v>
+      </c>
+      <c r="E105">
+        <v>62.0333</v>
+      </c>
+      <c r="F105">
+        <v>4.43333</v>
+      </c>
+      <c r="G105">
+        <v>9</v>
+      </c>
+      <c r="H105">
+        <v>15.6667</v>
+      </c>
+      <c r="I105">
+        <v>4.69999</v>
+      </c>
+      <c r="J105">
+        <v>9</v>
+      </c>
+      <c r="K105">
+        <v>7.43332</v>
+      </c>
+      <c r="L105">
+        <v>12.0333</v>
+      </c>
+      <c r="M105">
+        <v>7</v>
+      </c>
+      <c r="N105">
+        <v>8.39999</v>
+      </c>
+      <c r="O105">
+        <v>12.4</v>
+      </c>
+      <c r="P105">
+        <v>5</v>
+      </c>
+      <c r="Q105">
+        <v>15.0333</v>
+      </c>
+      <c r="R105">
+        <v>4.43333</v>
+      </c>
+      <c r="S105">
+        <v>1</v>
+      </c>
+      <c r="T105">
+        <v>7.89999</v>
+      </c>
+      <c r="U105">
+        <v>59.5999</v>
+      </c>
+      <c r="V105">
+        <v>1</v>
+      </c>
+      <c r="W105">
+        <v>0.966665</v>
+      </c>
+      <c r="X105">
+        <v>67.8999</v>
+      </c>
+      <c r="Y105">
+        <v>1</v>
+      </c>
+      <c r="Z105">
+        <v>3.56666</v>
+      </c>
+      <c r="AA105">
+        <v>6.53333</v>
+      </c>
+      <c r="AB105">
+        <v>0</v>
+      </c>
+      <c r="AC105">
+        <v>0</v>
+      </c>
+      <c r="AD105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE105">
+        <v>3</v>
+      </c>
+      <c r="AF105">
+        <v>2.7</v>
+      </c>
+      <c r="AG105">
+        <v>10.7667</v>
+      </c>
+      <c r="AH105">
+        <v>14.4364</v>
+      </c>
+      <c r="AI105">
+        <v>26158.8</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Trial   103</t>
+        </is>
+      </c>
+      <c r="B106">
+        <v>1090.99</v>
+      </c>
+      <c r="C106">
+        <v>10.2249</v>
+      </c>
+      <c r="D106">
+        <v>28</v>
+      </c>
+      <c r="E106">
+        <v>110.9</v>
+      </c>
+      <c r="F106">
+        <v>0.366666</v>
+      </c>
+      <c r="G106">
+        <v>16</v>
+      </c>
+      <c r="H106">
+        <v>34.4333</v>
+      </c>
+      <c r="I106">
+        <v>2.66666</v>
+      </c>
+      <c r="J106">
+        <v>10</v>
+      </c>
+      <c r="K106">
+        <v>15.4</v>
+      </c>
+      <c r="L106">
+        <v>13.1</v>
+      </c>
+      <c r="M106">
+        <v>12</v>
+      </c>
+      <c r="N106">
+        <v>17.5</v>
+      </c>
+      <c r="O106">
+        <v>0.366666</v>
+      </c>
+      <c r="P106">
+        <v>9</v>
+      </c>
+      <c r="Q106">
+        <v>18.4666</v>
+      </c>
+      <c r="R106">
+        <v>1.86666</v>
+      </c>
+      <c r="S106">
+        <v>4</v>
+      </c>
+      <c r="T106">
+        <v>6.23333</v>
+      </c>
+      <c r="U106">
+        <v>2.93333</v>
+      </c>
+      <c r="V106">
+        <v>2</v>
+      </c>
+      <c r="W106">
+        <v>1.8</v>
+      </c>
+      <c r="X106">
+        <v>9.26666</v>
+      </c>
+      <c r="Y106">
+        <v>1</v>
+      </c>
+      <c r="Z106">
+        <v>14.5333</v>
+      </c>
+      <c r="AA106">
+        <v>99.1999</v>
+      </c>
+      <c r="AB106">
+        <v>0</v>
+      </c>
+      <c r="AC106">
+        <v>0</v>
+      </c>
+      <c r="AD106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE106">
+        <v>4</v>
+      </c>
+      <c r="AF106">
+        <v>1.46667</v>
+      </c>
+      <c r="AG106">
+        <v>12.5</v>
+      </c>
+      <c r="AH106">
+        <v>14.2485</v>
+      </c>
+      <c r="AI106">
+        <v>46094.1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Trial   104</t>
+        </is>
+      </c>
+      <c r="B107">
+        <v>417.726</v>
+      </c>
+      <c r="C107">
+        <v>9.66214</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>43.3666</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>5</v>
+      </c>
+      <c r="H107">
+        <v>5.2</v>
+      </c>
+      <c r="I107">
+        <v>4.43333</v>
+      </c>
+      <c r="J107">
+        <v>1</v>
+      </c>
+      <c r="K107">
+        <v>4.43333</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107">
+        <v>1</v>
+      </c>
+      <c r="N107">
+        <v>6.26666</v>
+      </c>
+      <c r="O107">
+        <v>36.2333</v>
+      </c>
+      <c r="P107">
+        <v>1</v>
+      </c>
+      <c r="Q107">
+        <v>6.59999</v>
+      </c>
+      <c r="R107">
+        <v>27.3666</v>
+      </c>
+      <c r="S107">
+        <v>1</v>
+      </c>
+      <c r="T107">
+        <v>11.3667</v>
+      </c>
+      <c r="U107">
+        <v>15.5</v>
+      </c>
+      <c r="V107">
+        <v>0</v>
+      </c>
+      <c r="W107">
+        <v>0</v>
+      </c>
+      <c r="X107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y107">
+        <v>1</v>
+      </c>
+      <c r="Z107">
+        <v>9.29999</v>
+      </c>
+      <c r="AA107">
+        <v>5.39999</v>
+      </c>
+      <c r="AB107">
+        <v>0</v>
+      </c>
+      <c r="AC107">
+        <v>0</v>
+      </c>
+      <c r="AD107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE107">
+        <v>0</v>
+      </c>
+      <c r="AF107">
+        <v>0</v>
+      </c>
+      <c r="AG107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH107">
+        <v>20.6066</v>
+      </c>
+      <c r="AI107">
+        <v>26747.4</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Trial   105</t>
+        </is>
+      </c>
+      <c r="B108">
+        <v>940.208</v>
+      </c>
+      <c r="C108">
+        <v>14.4722</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>65.0999</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>14</v>
+      </c>
+      <c r="H108">
+        <v>15.1667</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>1</v>
+      </c>
+      <c r="K108">
+        <v>6.19999</v>
+      </c>
+      <c r="L108">
+        <v>43.8</v>
+      </c>
+      <c r="M108">
+        <v>3</v>
+      </c>
+      <c r="N108">
+        <v>10.1</v>
+      </c>
+      <c r="O108">
+        <v>2.4</v>
+      </c>
+      <c r="P108">
+        <v>1</v>
+      </c>
+      <c r="Q108">
+        <v>1.76666</v>
+      </c>
+      <c r="R108">
+        <v>7.29999</v>
+      </c>
+      <c r="S108">
+        <v>2</v>
+      </c>
+      <c r="T108">
+        <v>9.43332</v>
+      </c>
+      <c r="U108">
+        <v>17.4333</v>
+      </c>
+      <c r="V108">
+        <v>2</v>
+      </c>
+      <c r="W108">
+        <v>8.66666</v>
+      </c>
+      <c r="X108">
+        <v>0.033333</v>
+      </c>
+      <c r="Y108">
+        <v>2</v>
+      </c>
+      <c r="Z108">
+        <v>7.69999</v>
+      </c>
+      <c r="AA108">
+        <v>56.2666</v>
+      </c>
+      <c r="AB108">
+        <v>1</v>
+      </c>
+      <c r="AC108">
+        <v>3.6</v>
+      </c>
+      <c r="AD108">
+        <v>33.0333</v>
+      </c>
+      <c r="AE108">
+        <v>1</v>
+      </c>
+      <c r="AF108">
+        <v>2</v>
+      </c>
+      <c r="AG108">
+        <v>10.3</v>
+      </c>
+      <c r="AH108">
+        <v>16.2782</v>
+      </c>
+      <c r="AI108">
+        <v>31742.5</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Trial   106</t>
+        </is>
+      </c>
+      <c r="B109">
+        <v>348.143</v>
+      </c>
+      <c r="C109">
+        <v>9.05052</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>38.5</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109">
+        <v>5</v>
+      </c>
+      <c r="H109">
+        <v>5.23333</v>
+      </c>
+      <c r="I109">
+        <v>2.16666</v>
+      </c>
+      <c r="J109">
+        <v>1</v>
+      </c>
+      <c r="K109">
+        <v>6.59999</v>
+      </c>
+      <c r="L109">
+        <v>2.76666</v>
+      </c>
+      <c r="M109">
+        <v>1</v>
+      </c>
+      <c r="N109">
+        <v>7.29999</v>
+      </c>
+      <c r="O109">
+        <v>10.0333</v>
+      </c>
+      <c r="P109">
+        <v>0</v>
+      </c>
+      <c r="Q109">
+        <v>0</v>
+      </c>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S109">
+        <v>1</v>
+      </c>
+      <c r="T109">
+        <v>7.36666</v>
+      </c>
+      <c r="U109">
+        <v>19.1</v>
+      </c>
+      <c r="V109">
+        <v>0</v>
+      </c>
+      <c r="W109">
+        <v>0</v>
+      </c>
+      <c r="X109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y109">
+        <v>1</v>
+      </c>
+      <c r="Z109">
+        <v>9.63332</v>
+      </c>
+      <c r="AA109">
+        <v>28.3</v>
+      </c>
+      <c r="AB109">
+        <v>0</v>
+      </c>
+      <c r="AC109">
+        <v>0</v>
+      </c>
+      <c r="AD109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE109">
+        <v>1</v>
+      </c>
+      <c r="AF109">
+        <v>2.13333</v>
+      </c>
+      <c r="AG109">
+        <v>0</v>
+      </c>
+      <c r="AH109">
+        <v>18.7527</v>
+      </c>
+      <c r="AI109">
+        <v>21659.4</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Trial   107</t>
+        </is>
+      </c>
+      <c r="B110">
+        <v>628.822</v>
+      </c>
+      <c r="C110">
+        <v>13.2663</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>47.4333</v>
+      </c>
+      <c r="F110">
+        <v>0.099999</v>
+      </c>
+      <c r="G110">
+        <v>10</v>
+      </c>
+      <c r="H110">
+        <v>3.96666</v>
+      </c>
+      <c r="I110">
+        <v>0.099999</v>
+      </c>
+      <c r="J110">
+        <v>1</v>
+      </c>
+      <c r="K110">
+        <v>7.36666</v>
+      </c>
+      <c r="L110">
+        <v>6.29999</v>
+      </c>
+      <c r="M110">
+        <v>1</v>
+      </c>
+      <c r="N110">
+        <v>6.43333</v>
+      </c>
+      <c r="O110">
+        <v>14</v>
+      </c>
+      <c r="P110">
+        <v>1</v>
+      </c>
+      <c r="Q110">
+        <v>2.8</v>
+      </c>
+      <c r="R110">
+        <v>20.7666</v>
+      </c>
+      <c r="S110">
+        <v>1</v>
+      </c>
+      <c r="T110">
+        <v>7.49999</v>
+      </c>
+      <c r="U110">
+        <v>23.9333</v>
+      </c>
+      <c r="V110">
+        <v>2</v>
+      </c>
+      <c r="W110">
+        <v>4.43333</v>
+      </c>
+      <c r="X110">
+        <v>0.133333</v>
+      </c>
+      <c r="Y110">
+        <v>1</v>
+      </c>
+      <c r="Z110">
+        <v>11.6</v>
+      </c>
+      <c r="AA110">
+        <v>35.3666</v>
+      </c>
+      <c r="AB110">
+        <v>1</v>
+      </c>
+      <c r="AC110">
+        <v>1.46667</v>
+      </c>
+      <c r="AD110">
+        <v>2.2</v>
+      </c>
+      <c r="AE110">
+        <v>1</v>
+      </c>
+      <c r="AF110">
+        <v>1.73333</v>
+      </c>
+      <c r="AG110">
+        <v>4.16666</v>
+      </c>
+      <c r="AH110">
+        <v>21.5368</v>
+      </c>
+      <c r="AI110">
+        <v>30646.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>